<commit_message>
update demos files and version to 2.1.0
</commit_message>
<xml_diff>
--- a/src/assets/templates/heavydyn/PV Heavydyn Demo FR.xlsx
+++ b/src/assets/templates/heavydyn/PV Heavydyn Demo FR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spellevrault\Documents\Git\mvreport\src\MvrTester\Demo Heavydyn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spellevrault\Documents\Git\rapportxls\Template Mapview 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D810B4-DBD2-46CE-91C1-224F16FCE426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2333F4A1-0B91-47F3-B31A-F7A593864D76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10030" yWindow="3340" windowWidth="26670" windowHeight="16560" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9230" yWindow="4820" windowWidth="28800" windowHeight="15370" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RawData" sheetId="1" r:id="rId1"/>
@@ -1590,7 +1590,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="266">
+  <cellXfs count="272">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2000,6 +2000,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2105,11 +2111,8 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2240,6 +2243,12 @@
     <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2290,6 +2299,15 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8141,7 +8159,7 @@
   <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A7" zoomScale="85" zoomScaleNormal="115" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+      <selection activeCell="E28" sqref="E28:G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -8174,18 +8192,18 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="213" t="s">
+      <c r="E2" s="214" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="214"/>
-      <c r="G2" s="214"/>
-      <c r="H2" s="214"/>
-      <c r="I2" s="214"/>
-      <c r="J2" s="214"/>
-      <c r="K2" s="214"/>
-      <c r="L2" s="214"/>
-      <c r="M2" s="214"/>
-      <c r="N2" s="214"/>
+      <c r="F2" s="215"/>
+      <c r="G2" s="215"/>
+      <c r="H2" s="215"/>
+      <c r="I2" s="215"/>
+      <c r="J2" s="215"/>
+      <c r="K2" s="215"/>
+      <c r="L2" s="215"/>
+      <c r="M2" s="215"/>
+      <c r="N2" s="215"/>
       <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -8194,14 +8212,14 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="215"/>
-      <c r="G3" s="215"/>
-      <c r="H3" s="215"/>
-      <c r="I3" s="215"/>
-      <c r="J3" s="215"/>
-      <c r="K3" s="215"/>
-      <c r="L3" s="215"/>
-      <c r="M3" s="215"/>
+      <c r="F3" s="216"/>
+      <c r="G3" s="216"/>
+      <c r="H3" s="216"/>
+      <c r="I3" s="216"/>
+      <c r="J3" s="216"/>
+      <c r="K3" s="216"/>
+      <c r="L3" s="216"/>
+      <c r="M3" s="216"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
@@ -8258,9 +8276,9 @@
     </row>
     <row r="7" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
-      <c r="B7" s="216"/>
-      <c r="C7" s="216"/>
-      <c r="D7" s="216"/>
+      <c r="B7" s="217"/>
+      <c r="C7" s="217"/>
+      <c r="D7" s="217"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -8275,11 +8293,11 @@
     </row>
     <row r="8" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="217" t="s">
+      <c r="B8" s="218" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="183"/>
-      <c r="D8" s="183"/>
+      <c r="C8" s="185"/>
+      <c r="D8" s="185"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -8293,11 +8311,11 @@
       <c r="O8" s="2"/>
     </row>
     <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="218"/>
-      <c r="B9" s="218"/>
-      <c r="C9" s="218"/>
-      <c r="D9" s="218"/>
-      <c r="E9" s="218"/>
+      <c r="A9" s="219"/>
+      <c r="B9" s="219"/>
+      <c r="C9" s="219"/>
+      <c r="D9" s="219"/>
+      <c r="E9" s="219"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="5"/>
@@ -8310,28 +8328,28 @@
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="219"/>
-      <c r="B10" s="219"/>
-      <c r="C10" s="219"/>
-      <c r="D10" s="219"/>
-      <c r="E10" s="219"/>
+      <c r="A10" s="220"/>
+      <c r="B10" s="220"/>
+      <c r="C10" s="220"/>
+      <c r="D10" s="220"/>
+      <c r="E10" s="220"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="5"/>
       <c r="I10" s="6"/>
-      <c r="J10" s="220"/>
-      <c r="K10" s="220"/>
-      <c r="L10" s="220"/>
+      <c r="J10" s="221"/>
+      <c r="K10" s="221"/>
+      <c r="L10" s="221"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:15" ht="1.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="208"/>
-      <c r="B11" s="208"/>
-      <c r="C11" s="208"/>
-      <c r="D11" s="208"/>
-      <c r="E11" s="208"/>
+      <c r="A11" s="209"/>
+      <c r="B11" s="209"/>
+      <c r="C11" s="209"/>
+      <c r="D11" s="209"/>
+      <c r="E11" s="209"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
@@ -8345,57 +8363,57 @@
     </row>
     <row r="12" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
-      <c r="B12" s="209" t="s">
+      <c r="B12" s="210" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="209"/>
-      <c r="D12" s="209"/>
-      <c r="E12" s="209"/>
-      <c r="F12" s="209"/>
-      <c r="G12" s="209"/>
-      <c r="H12" s="209"/>
-      <c r="I12" s="209"/>
-      <c r="J12" s="209"/>
-      <c r="K12" s="209"/>
-      <c r="L12" s="209"/>
-      <c r="M12" s="209"/>
-      <c r="N12" s="209"/>
+      <c r="C12" s="210"/>
+      <c r="D12" s="210"/>
+      <c r="E12" s="210"/>
+      <c r="F12" s="210"/>
+      <c r="G12" s="210"/>
+      <c r="H12" s="210"/>
+      <c r="I12" s="210"/>
+      <c r="J12" s="210"/>
+      <c r="K12" s="210"/>
+      <c r="L12" s="210"/>
+      <c r="M12" s="210"/>
+      <c r="N12" s="210"/>
       <c r="O12" s="2"/>
     </row>
     <row r="13" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
-      <c r="B13" s="210" t="s">
+      <c r="B13" s="211" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="210"/>
-      <c r="D13" s="210"/>
-      <c r="E13" s="210"/>
-      <c r="F13" s="210"/>
-      <c r="G13" s="210"/>
-      <c r="H13" s="210"/>
-      <c r="I13" s="210"/>
-      <c r="J13" s="210"/>
-      <c r="K13" s="210"/>
-      <c r="L13" s="210"/>
-      <c r="M13" s="210"/>
-      <c r="N13" s="210"/>
+      <c r="C13" s="211"/>
+      <c r="D13" s="211"/>
+      <c r="E13" s="211"/>
+      <c r="F13" s="211"/>
+      <c r="G13" s="211"/>
+      <c r="H13" s="211"/>
+      <c r="I13" s="211"/>
+      <c r="J13" s="211"/>
+      <c r="K13" s="211"/>
+      <c r="L13" s="211"/>
+      <c r="M13" s="211"/>
+      <c r="N13" s="211"/>
       <c r="O13" s="2"/>
     </row>
     <row r="14" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
-      <c r="B14" s="210"/>
-      <c r="C14" s="210"/>
-      <c r="D14" s="210"/>
-      <c r="E14" s="210"/>
-      <c r="F14" s="210"/>
-      <c r="G14" s="210"/>
-      <c r="H14" s="210"/>
-      <c r="I14" s="210"/>
-      <c r="J14" s="210"/>
-      <c r="K14" s="210"/>
-      <c r="L14" s="210"/>
-      <c r="M14" s="210"/>
-      <c r="N14" s="210"/>
+      <c r="B14" s="211"/>
+      <c r="C14" s="211"/>
+      <c r="D14" s="211"/>
+      <c r="E14" s="211"/>
+      <c r="F14" s="211"/>
+      <c r="G14" s="211"/>
+      <c r="H14" s="211"/>
+      <c r="I14" s="211"/>
+      <c r="J14" s="211"/>
+      <c r="K14" s="211"/>
+      <c r="L14" s="211"/>
+      <c r="M14" s="211"/>
+      <c r="N14" s="211"/>
       <c r="O14" s="2"/>
     </row>
     <row r="15" spans="1:15" ht="6.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -8417,21 +8435,21 @@
     </row>
     <row r="16" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
-      <c r="B16" s="186" t="s">
+      <c r="B16" s="188" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="187"/>
-      <c r="D16" s="187"/>
-      <c r="E16" s="187"/>
-      <c r="F16" s="187"/>
-      <c r="G16" s="187"/>
-      <c r="H16" s="187"/>
-      <c r="I16" s="187"/>
-      <c r="J16" s="187"/>
-      <c r="K16" s="187"/>
-      <c r="L16" s="187"/>
-      <c r="M16" s="187"/>
-      <c r="N16" s="188"/>
+      <c r="C16" s="189"/>
+      <c r="D16" s="189"/>
+      <c r="E16" s="189"/>
+      <c r="F16" s="189"/>
+      <c r="G16" s="189"/>
+      <c r="H16" s="189"/>
+      <c r="I16" s="189"/>
+      <c r="J16" s="189"/>
+      <c r="K16" s="189"/>
+      <c r="L16" s="189"/>
+      <c r="M16" s="189"/>
+      <c r="N16" s="190"/>
       <c r="O16" s="2"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -8441,24 +8459,24 @@
       <c r="D17" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="202" t="e">
+      <c r="E17" s="204" t="e">
         <f>IF(Project_Name="","",Project_Name)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F17" s="202"/>
-      <c r="G17" s="202"/>
-      <c r="H17" s="202"/>
+      <c r="F17" s="204"/>
+      <c r="G17" s="204"/>
+      <c r="H17" s="204"/>
       <c r="I17" s="31"/>
       <c r="J17" s="31"/>
       <c r="K17" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="L17" s="206">
+      <c r="L17" s="207">
         <f ca="1">TODAY()</f>
-        <v>44984</v>
-      </c>
-      <c r="M17" s="206"/>
-      <c r="N17" s="206"/>
+        <v>44993</v>
+      </c>
+      <c r="M17" s="207"/>
+      <c r="N17" s="207"/>
       <c r="O17" s="2"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -8468,24 +8486,24 @@
       <c r="D18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="203" t="e">
+      <c r="E18" s="205" t="e">
         <f>IF(Project_Town="","",Project_Town)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F18" s="203"/>
-      <c r="G18" s="203"/>
-      <c r="H18" s="203"/>
+      <c r="F18" s="205"/>
+      <c r="G18" s="205"/>
+      <c r="H18" s="205"/>
       <c r="I18" s="34"/>
       <c r="J18" s="35"/>
       <c r="K18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L18" s="211" t="e">
+      <c r="L18" s="212" t="e">
         <f>IF(Project_Project="","", Project_Project)</f>
         <v>#NAME?</v>
       </c>
-      <c r="M18" s="211"/>
-      <c r="N18" s="211"/>
+      <c r="M18" s="212"/>
+      <c r="N18" s="212"/>
       <c r="O18" s="2"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -8495,24 +8513,24 @@
       <c r="D19" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="199" t="e">
+      <c r="E19" s="201" t="e">
         <f>IF(Project_Customer="","",Project_Customer)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F19" s="199"/>
-      <c r="G19" s="199"/>
-      <c r="H19" s="199"/>
+      <c r="F19" s="201"/>
+      <c r="G19" s="201"/>
+      <c r="H19" s="201"/>
       <c r="I19" s="39"/>
       <c r="J19" s="39"/>
       <c r="K19" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="L19" s="212" t="e">
+      <c r="L19" s="213" t="e">
         <f xml:space="preserve"> IF(Project_Contact="","",Project_Contact)</f>
         <v>#NAME?</v>
       </c>
-      <c r="M19" s="212"/>
-      <c r="N19" s="212"/>
+      <c r="M19" s="213"/>
+      <c r="N19" s="213"/>
       <c r="O19" s="2"/>
     </row>
     <row r="20" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -8534,21 +8552,21 @@
     </row>
     <row r="21" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
-      <c r="B21" s="186" t="s">
+      <c r="B21" s="188" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="187"/>
-      <c r="D21" s="187"/>
-      <c r="E21" s="187"/>
-      <c r="F21" s="187"/>
-      <c r="G21" s="187"/>
-      <c r="H21" s="187"/>
-      <c r="I21" s="187"/>
-      <c r="J21" s="187"/>
-      <c r="K21" s="187"/>
-      <c r="L21" s="187"/>
-      <c r="M21" s="187"/>
-      <c r="N21" s="188"/>
+      <c r="C21" s="189"/>
+      <c r="D21" s="189"/>
+      <c r="E21" s="189"/>
+      <c r="F21" s="189"/>
+      <c r="G21" s="189"/>
+      <c r="H21" s="189"/>
+      <c r="I21" s="189"/>
+      <c r="J21" s="189"/>
+      <c r="K21" s="189"/>
+      <c r="L21" s="189"/>
+      <c r="M21" s="189"/>
+      <c r="N21" s="190"/>
       <c r="O21" s="2"/>
     </row>
     <row r="22" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -8558,24 +8576,24 @@
       <c r="D22" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="202" t="e">
+      <c r="E22" s="204" t="e">
         <f>IF(Project_Site="","",Project_Site)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F22" s="202"/>
-      <c r="G22" s="202"/>
+      <c r="F22" s="204"/>
+      <c r="G22" s="204"/>
       <c r="H22" s="31"/>
       <c r="I22" s="31"/>
       <c r="J22" s="31"/>
       <c r="K22" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="L22" s="206" t="e">
+      <c r="L22" s="207" t="e">
         <f>IF(Report_Date="","",Report_Date)</f>
         <v>#NAME?</v>
       </c>
-      <c r="M22" s="202"/>
-      <c r="N22" s="207"/>
+      <c r="M22" s="204"/>
+      <c r="N22" s="208"/>
       <c r="O22" s="2"/>
     </row>
     <row r="23" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -8585,24 +8603,24 @@
       <c r="D23" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="203" t="e">
+      <c r="E23" s="205" t="e">
         <f>IF(Report_Lane="","",Report_Lane)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F23" s="203"/>
-      <c r="G23" s="203"/>
+      <c r="F23" s="205"/>
+      <c r="G23" s="205"/>
       <c r="H23" s="40"/>
       <c r="I23" s="40"/>
       <c r="J23" s="40"/>
       <c r="K23" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="L23" s="196" t="e" cm="1">
+      <c r="L23" s="198" t="e" cm="1">
         <f t="array" ref="L23">IF(Report_Part="","",Report_Part)</f>
         <v>#NAME?</v>
       </c>
-      <c r="M23" s="197"/>
-      <c r="N23" s="198"/>
+      <c r="M23" s="199"/>
+      <c r="N23" s="200"/>
       <c r="O23" s="19"/>
     </row>
     <row r="24" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -8612,19 +8630,19 @@
       <c r="D24" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="199" t="e">
+      <c r="E24" s="201" t="e">
         <f>IF(Report_Direction="","",Report_Direction)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F24" s="199"/>
-      <c r="G24" s="199"/>
+      <c r="F24" s="201"/>
+      <c r="G24" s="201"/>
       <c r="H24" s="39"/>
       <c r="I24" s="39"/>
       <c r="J24" s="39"/>
       <c r="K24" s="38"/>
-      <c r="L24" s="200"/>
-      <c r="M24" s="200"/>
-      <c r="N24" s="201"/>
+      <c r="L24" s="202"/>
+      <c r="M24" s="202"/>
+      <c r="N24" s="203"/>
       <c r="O24" s="2"/>
     </row>
     <row r="25" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -8646,21 +8664,21 @@
     </row>
     <row r="26" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="16"/>
-      <c r="B26" s="186" t="s">
+      <c r="B26" s="188" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="187"/>
-      <c r="D26" s="187"/>
-      <c r="E26" s="187"/>
-      <c r="F26" s="187"/>
-      <c r="G26" s="187"/>
-      <c r="H26" s="187"/>
-      <c r="I26" s="187"/>
-      <c r="J26" s="187"/>
-      <c r="K26" s="187"/>
-      <c r="L26" s="187"/>
-      <c r="M26" s="187"/>
-      <c r="N26" s="188"/>
+      <c r="C26" s="189"/>
+      <c r="D26" s="189"/>
+      <c r="E26" s="189"/>
+      <c r="F26" s="189"/>
+      <c r="G26" s="189"/>
+      <c r="H26" s="189"/>
+      <c r="I26" s="189"/>
+      <c r="J26" s="189"/>
+      <c r="K26" s="189"/>
+      <c r="L26" s="189"/>
+      <c r="M26" s="189"/>
+      <c r="N26" s="190"/>
       <c r="O26" s="2"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
@@ -8670,24 +8688,24 @@
       <c r="D27" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="E27" s="202" t="e">
+      <c r="E27" s="204" t="e">
         <f>IF(Platform_Type="","",Platform_Type)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F27" s="202"/>
-      <c r="G27" s="202"/>
+      <c r="F27" s="204"/>
+      <c r="G27" s="204"/>
       <c r="H27" s="29"/>
       <c r="I27" s="31"/>
       <c r="J27" s="31"/>
       <c r="K27" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="L27" s="9" t="e">
+      <c r="L27" s="169" t="e">
         <f>ROUND(AVERAGE(Pi_Tsurf),1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="M27" s="9"/>
-      <c r="N27" s="41"/>
+      <c r="M27" s="169"/>
+      <c r="N27" s="170"/>
       <c r="O27" s="2"/>
     </row>
     <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -8697,24 +8715,24 @@
       <c r="D28" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E28" s="203" t="e">
+      <c r="E28" s="205" t="e">
         <f>IF(Platform_Layer="","",Platform_Layer)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F28" s="203"/>
-      <c r="G28" s="203"/>
+      <c r="F28" s="205"/>
+      <c r="G28" s="205"/>
       <c r="H28" s="40"/>
       <c r="I28" s="40"/>
       <c r="J28" s="40"/>
       <c r="K28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L28" s="9" t="e">
+      <c r="L28" s="169" t="e">
         <f>ROUND(AVERAGE(Pi_Tair),1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="M28" s="9"/>
-      <c r="N28" s="41"/>
+      <c r="M28" s="169"/>
+      <c r="N28" s="170"/>
       <c r="O28" s="19"/>
     </row>
     <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -8724,24 +8742,24 @@
       <c r="D29" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E29" s="197" t="e">
+      <c r="E29" s="199" t="e">
         <f>IF(Platform_Material="","",Platform_Material)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F29" s="197"/>
-      <c r="G29" s="197"/>
+      <c r="F29" s="199"/>
+      <c r="G29" s="199"/>
       <c r="H29" s="40"/>
       <c r="I29" s="40"/>
       <c r="J29" s="40"/>
       <c r="K29" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="L29" s="204" t="e">
+      <c r="L29" s="205" t="e">
         <f>IF(Report_Weather="","",Report_Weather)</f>
         <v>#NAME?</v>
       </c>
-      <c r="M29" s="204"/>
-      <c r="N29" s="205"/>
+      <c r="M29" s="205"/>
+      <c r="N29" s="206"/>
       <c r="O29" s="19"/>
     </row>
     <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -8819,21 +8837,21 @@
     </row>
     <row r="33" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
-      <c r="B33" s="186" t="s">
+      <c r="B33" s="188" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="187"/>
-      <c r="D33" s="187"/>
-      <c r="E33" s="187"/>
-      <c r="F33" s="187"/>
-      <c r="G33" s="187"/>
-      <c r="H33" s="187"/>
-      <c r="I33" s="187"/>
-      <c r="J33" s="187"/>
-      <c r="K33" s="187"/>
-      <c r="L33" s="187"/>
-      <c r="M33" s="187"/>
-      <c r="N33" s="188"/>
+      <c r="C33" s="189"/>
+      <c r="D33" s="189"/>
+      <c r="E33" s="189"/>
+      <c r="F33" s="189"/>
+      <c r="G33" s="189"/>
+      <c r="H33" s="189"/>
+      <c r="I33" s="189"/>
+      <c r="J33" s="189"/>
+      <c r="K33" s="189"/>
+      <c r="L33" s="189"/>
+      <c r="M33" s="189"/>
+      <c r="N33" s="190"/>
       <c r="O33" s="2"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
@@ -8843,24 +8861,24 @@
       <c r="D34" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="E34" s="169" t="e" cm="1">
+      <c r="E34" s="171" t="e" cm="1">
         <f t="array" ref="E34">IF(Hardware_SerialNumber="","","Heavydyn " &amp; Hardware_SerialNumber)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F34" s="169"/>
-      <c r="G34" s="169"/>
+      <c r="F34" s="171"/>
+      <c r="G34" s="171"/>
       <c r="H34" s="45"/>
       <c r="I34" s="45"/>
       <c r="J34" s="45"/>
       <c r="K34" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="L34" s="170" t="e" cm="1">
+      <c r="L34" s="172" t="e" cm="1">
         <f t="array" ref="L34">IF(Hardware_CertificateStart="","",Hardware_CertificateStart)</f>
         <v>#NAME?</v>
       </c>
-      <c r="M34" s="170"/>
-      <c r="N34" s="171"/>
+      <c r="M34" s="172"/>
+      <c r="N34" s="173"/>
       <c r="O34" s="2"/>
     </row>
     <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -8882,45 +8900,45 @@
     </row>
     <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="18"/>
-      <c r="B36" s="186" t="s">
+      <c r="B36" s="188" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="187"/>
-      <c r="D36" s="187"/>
-      <c r="E36" s="187"/>
-      <c r="F36" s="187"/>
-      <c r="G36" s="187"/>
-      <c r="H36" s="187"/>
-      <c r="I36" s="187"/>
-      <c r="J36" s="187"/>
-      <c r="K36" s="187"/>
-      <c r="L36" s="187"/>
-      <c r="M36" s="187"/>
-      <c r="N36" s="188"/>
+      <c r="C36" s="189"/>
+      <c r="D36" s="189"/>
+      <c r="E36" s="189"/>
+      <c r="F36" s="189"/>
+      <c r="G36" s="189"/>
+      <c r="H36" s="189"/>
+      <c r="I36" s="189"/>
+      <c r="J36" s="189"/>
+      <c r="K36" s="189"/>
+      <c r="L36" s="189"/>
+      <c r="M36" s="189"/>
+      <c r="N36" s="190"/>
       <c r="O36" s="19"/>
     </row>
     <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="18"/>
-      <c r="B37" s="189"/>
-      <c r="C37" s="190"/>
-      <c r="D37" s="191" t="s">
+      <c r="B37" s="191"/>
+      <c r="C37" s="192"/>
+      <c r="D37" s="193" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="191"/>
-      <c r="F37" s="191"/>
-      <c r="G37" s="191" t="e" cm="1">
+      <c r="E37" s="193"/>
+      <c r="F37" s="193"/>
+      <c r="G37" s="193" t="e" cm="1">
         <f t="array" ref="G37">"Valeur corrigées (" &amp; Unit_Force_Unit &amp; ", " &amp;Unit_Deflection_Unit &amp; ")"</f>
         <v>#NAME?</v>
       </c>
-      <c r="H37" s="191"/>
-      <c r="I37" s="191"/>
-      <c r="J37" s="191"/>
-      <c r="K37" s="191"/>
-      <c r="L37" s="191"/>
-      <c r="M37" s="192" t="s">
+      <c r="H37" s="193"/>
+      <c r="I37" s="193"/>
+      <c r="J37" s="193"/>
+      <c r="K37" s="193"/>
+      <c r="L37" s="193"/>
+      <c r="M37" s="194" t="s">
         <v>42</v>
       </c>
-      <c r="N37" s="193"/>
+      <c r="N37" s="195"/>
       <c r="O37" s="19"/>
     </row>
     <row r="38" spans="1:15" ht="34" customHeight="1" x14ac:dyDescent="0.3">
@@ -8958,8 +8976,8 @@
       <c r="L38" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="M38" s="194"/>
-      <c r="N38" s="195"/>
+      <c r="M38" s="196"/>
+      <c r="N38" s="197"/>
       <c r="O38" s="19"/>
     </row>
     <row r="39" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -9007,8 +9025,8 @@
         <f t="array" ref="L39">IFERROR(Z1_CharacteristicDeflection,"")</f>
         <v/>
       </c>
-      <c r="M39" s="223"/>
-      <c r="N39" s="224"/>
+      <c r="M39" s="224"/>
+      <c r="N39" s="225"/>
       <c r="O39" s="19"/>
     </row>
     <row r="40" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -9056,8 +9074,8 @@
         <f t="array" ref="L40">IFERROR(Z2_CharacteristicDeflection,"")</f>
         <v/>
       </c>
-      <c r="M40" s="225"/>
-      <c r="N40" s="226"/>
+      <c r="M40" s="226"/>
+      <c r="N40" s="227"/>
       <c r="O40" s="19"/>
     </row>
     <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -9105,8 +9123,8 @@
         <f t="array" ref="L41">IFERROR(Z3_CharacteristicDeflection,"")</f>
         <v/>
       </c>
-      <c r="M41" s="225"/>
-      <c r="N41" s="226"/>
+      <c r="M41" s="226"/>
+      <c r="N41" s="227"/>
       <c r="O41" s="19"/>
     </row>
     <row r="42" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -9154,8 +9172,8 @@
         <f t="array" ref="L42">IFERROR(Z4_CharacteristicDeflection,"")</f>
         <v/>
       </c>
-      <c r="M42" s="225"/>
-      <c r="N42" s="226"/>
+      <c r="M42" s="226"/>
+      <c r="N42" s="227"/>
       <c r="O42" s="19"/>
     </row>
     <row r="43" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -9203,8 +9221,8 @@
         <f t="array" ref="L43">IFERROR(Z5_CharacteristicDeflection,"")</f>
         <v/>
       </c>
-      <c r="M43" s="225"/>
-      <c r="N43" s="226"/>
+      <c r="M43" s="226"/>
+      <c r="N43" s="227"/>
       <c r="O43" s="19"/>
     </row>
     <row r="44" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -9252,8 +9270,8 @@
         <f t="array" ref="L44">IFERROR(Z6_CharacteristicDeflection,"")</f>
         <v/>
       </c>
-      <c r="M44" s="221"/>
-      <c r="N44" s="222"/>
+      <c r="M44" s="222"/>
+      <c r="N44" s="223"/>
       <c r="O44" s="19"/>
     </row>
     <row r="45" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -9298,57 +9316,57 @@
       <c r="C47" s="21"/>
       <c r="D47" s="22"/>
       <c r="E47" s="21"/>
-      <c r="F47" s="176" t="s">
+      <c r="F47" s="178" t="s">
         <v>31</v>
       </c>
-      <c r="G47" s="176"/>
-      <c r="H47" s="176"/>
-      <c r="I47" s="176"/>
-      <c r="J47" s="176"/>
+      <c r="G47" s="178"/>
+      <c r="H47" s="178"/>
+      <c r="I47" s="178"/>
+      <c r="J47" s="178"/>
       <c r="K47" s="10"/>
-      <c r="L47" s="177" t="s">
+      <c r="L47" s="179" t="s">
         <v>32</v>
       </c>
-      <c r="M47" s="177"/>
-      <c r="N47" s="178"/>
+      <c r="M47" s="179"/>
+      <c r="N47" s="180"/>
       <c r="O47" s="2"/>
     </row>
     <row r="48" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
-      <c r="B48" s="179" t="e">
+      <c r="B48" s="181" t="e">
         <f>IF(PVs_Commentaire="","",PVs_Commentaire)</f>
         <v>#NAME?</v>
       </c>
-      <c r="C48" s="180"/>
-      <c r="D48" s="180"/>
-      <c r="E48" s="180"/>
-      <c r="F48" s="183" t="e">
+      <c r="C48" s="182"/>
+      <c r="D48" s="182"/>
+      <c r="E48" s="182"/>
+      <c r="F48" s="185" t="e">
         <f>IF(PVs_Operateur="","",PVs_Operateur)</f>
         <v>#NAME?</v>
       </c>
-      <c r="G48" s="183"/>
-      <c r="H48" s="183"/>
-      <c r="I48" s="183"/>
-      <c r="J48" s="183"/>
+      <c r="G48" s="185"/>
+      <c r="H48" s="185"/>
+      <c r="I48" s="185"/>
+      <c r="J48" s="185"/>
       <c r="K48" s="2"/>
-      <c r="L48" s="184"/>
-      <c r="M48" s="184"/>
-      <c r="N48" s="185"/>
+      <c r="L48" s="186"/>
+      <c r="M48" s="186"/>
+      <c r="N48" s="187"/>
       <c r="O48" s="2"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
-      <c r="B49" s="179"/>
-      <c r="C49" s="180"/>
-      <c r="D49" s="180"/>
-      <c r="E49" s="180"/>
-      <c r="F49" s="183" t="s">
+      <c r="B49" s="181"/>
+      <c r="C49" s="182"/>
+      <c r="D49" s="182"/>
+      <c r="E49" s="182"/>
+      <c r="F49" s="185" t="s">
         <v>33</v>
       </c>
-      <c r="G49" s="183"/>
-      <c r="H49" s="183"/>
-      <c r="I49" s="183"/>
-      <c r="J49" s="183"/>
+      <c r="G49" s="185"/>
+      <c r="H49" s="185"/>
+      <c r="I49" s="185"/>
+      <c r="J49" s="185"/>
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
@@ -9357,10 +9375,10 @@
     </row>
     <row r="50" spans="1:15" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
-      <c r="B50" s="181"/>
-      <c r="C50" s="182"/>
-      <c r="D50" s="182"/>
-      <c r="E50" s="182"/>
+      <c r="B50" s="183"/>
+      <c r="C50" s="184"/>
+      <c r="D50" s="184"/>
+      <c r="E50" s="184"/>
       <c r="F50" s="24"/>
       <c r="G50" s="14"/>
       <c r="H50" s="14"/>
@@ -9394,20 +9412,20 @@
       <c r="B52" s="27"/>
       <c r="C52" s="27"/>
       <c r="D52" s="27"/>
-      <c r="E52" s="172" t="s">
+      <c r="E52" s="174" t="s">
         <v>39</v>
       </c>
-      <c r="F52" s="172"/>
-      <c r="G52" s="172"/>
-      <c r="H52" s="172"/>
-      <c r="I52" s="172"/>
-      <c r="J52" s="172"/>
-      <c r="K52" s="172"/>
-      <c r="L52" s="172"/>
-      <c r="M52" s="173" t="s">
+      <c r="F52" s="174"/>
+      <c r="G52" s="174"/>
+      <c r="H52" s="174"/>
+      <c r="I52" s="174"/>
+      <c r="J52" s="174"/>
+      <c r="K52" s="174"/>
+      <c r="L52" s="174"/>
+      <c r="M52" s="175" t="s">
         <v>34</v>
       </c>
-      <c r="N52" s="173"/>
+      <c r="N52" s="175"/>
       <c r="O52" s="2"/>
     </row>
     <row r="53" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -9415,18 +9433,18 @@
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
-      <c r="E53" s="175" t="s">
+      <c r="E53" s="177" t="s">
         <v>40</v>
       </c>
-      <c r="F53" s="175"/>
-      <c r="G53" s="175"/>
-      <c r="H53" s="175"/>
-      <c r="I53" s="175"/>
-      <c r="J53" s="175"/>
-      <c r="K53" s="175"/>
-      <c r="L53" s="175"/>
-      <c r="M53" s="174"/>
-      <c r="N53" s="174"/>
+      <c r="F53" s="177"/>
+      <c r="G53" s="177"/>
+      <c r="H53" s="177"/>
+      <c r="I53" s="177"/>
+      <c r="J53" s="177"/>
+      <c r="K53" s="177"/>
+      <c r="L53" s="177"/>
+      <c r="M53" s="176"/>
+      <c r="N53" s="176"/>
       <c r="O53" s="2"/>
     </row>
   </sheetData>
@@ -9543,34 +9561,34 @@
       <c r="X1" s="2"/>
     </row>
     <row r="2" spans="1:24" s="2" customFormat="1" ht="26.15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="J2" s="248" t="s">
+      <c r="J2" s="249" t="s">
         <v>53</v>
       </c>
-      <c r="K2" s="248"/>
-      <c r="L2" s="248"/>
-      <c r="M2" s="248"/>
-      <c r="N2" s="248"/>
-      <c r="O2" s="248"/>
-      <c r="P2" s="248"/>
-      <c r="Q2" s="248"/>
-      <c r="R2" s="248"/>
-      <c r="S2" s="248"/>
-      <c r="T2" s="248"/>
+      <c r="K2" s="249"/>
+      <c r="L2" s="249"/>
+      <c r="M2" s="249"/>
+      <c r="N2" s="249"/>
+      <c r="O2" s="249"/>
+      <c r="P2" s="249"/>
+      <c r="Q2" s="249"/>
+      <c r="R2" s="249"/>
+      <c r="S2" s="249"/>
+      <c r="T2" s="249"/>
     </row>
     <row r="3" spans="1:24" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="J3" s="215" t="s">
+      <c r="J3" s="216" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="215"/>
-      <c r="L3" s="215"/>
-      <c r="M3" s="215"/>
-      <c r="N3" s="215"/>
-      <c r="O3" s="215"/>
-      <c r="P3" s="215"/>
-      <c r="Q3" s="215"/>
-      <c r="R3" s="215"/>
-      <c r="S3" s="215"/>
-      <c r="T3" s="215"/>
+      <c r="K3" s="216"/>
+      <c r="L3" s="216"/>
+      <c r="M3" s="216"/>
+      <c r="N3" s="216"/>
+      <c r="O3" s="216"/>
+      <c r="P3" s="216"/>
+      <c r="Q3" s="216"/>
+      <c r="R3" s="216"/>
+      <c r="S3" s="216"/>
+      <c r="T3" s="216"/>
     </row>
     <row r="4" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
@@ -9599,17 +9617,17 @@
       <c r="X4" s="2"/>
     </row>
     <row r="5" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="218"/>
-      <c r="B5" s="218"/>
-      <c r="C5" s="218"/>
-      <c r="D5" s="218"/>
-      <c r="E5" s="218"/>
-      <c r="F5" s="218"/>
-      <c r="G5" s="218"/>
-      <c r="H5" s="218"/>
-      <c r="I5" s="218"/>
-      <c r="J5" s="218"/>
-      <c r="K5" s="218"/>
+      <c r="A5" s="219"/>
+      <c r="B5" s="219"/>
+      <c r="C5" s="219"/>
+      <c r="D5" s="219"/>
+      <c r="E5" s="219"/>
+      <c r="F5" s="219"/>
+      <c r="G5" s="219"/>
+      <c r="H5" s="219"/>
+      <c r="I5" s="219"/>
+      <c r="J5" s="219"/>
+      <c r="K5" s="219"/>
       <c r="L5" s="59"/>
       <c r="M5" s="59"/>
       <c r="N5" s="59"/>
@@ -9626,41 +9644,41 @@
     </row>
     <row r="6" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
-      <c r="B6" s="186" t="e" cm="1">
+      <c r="B6" s="188" t="e" cm="1">
         <f t="array" ref="B6" xml:space="preserve"> "INFORMATIONS ZONE " &amp; Zi_Name</f>
         <v>#NAME?</v>
       </c>
-      <c r="C6" s="187"/>
-      <c r="D6" s="187"/>
-      <c r="E6" s="187"/>
-      <c r="F6" s="187"/>
-      <c r="G6" s="187"/>
-      <c r="H6" s="187"/>
-      <c r="I6" s="187"/>
-      <c r="J6" s="187"/>
-      <c r="K6" s="187"/>
-      <c r="L6" s="187"/>
-      <c r="M6" s="187"/>
-      <c r="N6" s="187"/>
-      <c r="O6" s="187"/>
-      <c r="P6" s="187"/>
-      <c r="Q6" s="187"/>
-      <c r="R6" s="187"/>
-      <c r="S6" s="187"/>
-      <c r="T6" s="187"/>
-      <c r="U6" s="187"/>
-      <c r="V6" s="187"/>
-      <c r="W6" s="188"/>
+      <c r="C6" s="189"/>
+      <c r="D6" s="189"/>
+      <c r="E6" s="189"/>
+      <c r="F6" s="189"/>
+      <c r="G6" s="189"/>
+      <c r="H6" s="189"/>
+      <c r="I6" s="189"/>
+      <c r="J6" s="189"/>
+      <c r="K6" s="189"/>
+      <c r="L6" s="189"/>
+      <c r="M6" s="189"/>
+      <c r="N6" s="189"/>
+      <c r="O6" s="189"/>
+      <c r="P6" s="189"/>
+      <c r="Q6" s="189"/>
+      <c r="R6" s="189"/>
+      <c r="S6" s="189"/>
+      <c r="T6" s="189"/>
+      <c r="U6" s="189"/>
+      <c r="V6" s="189"/>
+      <c r="W6" s="190"/>
       <c r="X6" s="2"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
-      <c r="B7" s="249" t="e">
+      <c r="B7" s="252" t="e">
         <f>IF(CorrectionParameters_Load_Active,"Forces corrigées à :","Forces non corrigées")</f>
         <v>#NAME?</v>
       </c>
-      <c r="C7" s="250"/>
-      <c r="D7" s="250"/>
+      <c r="C7" s="253"/>
+      <c r="D7" s="253"/>
       <c r="E7" s="29" t="e">
         <f>IF(CorrectionParameters_Load_Active,IF(CorrectionParameters_Load_LoadReferenceSource="Sequence",DropSequence_Drop3_Value,CorrectionParameters_Load_CustomValue),"")</f>
         <v>#NAME?</v>
@@ -9689,23 +9707,23 @@
       <c r="S7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="T7" s="204" t="e">
+      <c r="T7" s="250" t="e">
         <f>IF(Project_Project="","", Project_Project)</f>
         <v>#NAME?</v>
       </c>
-      <c r="U7" s="204"/>
-      <c r="V7" s="204"/>
-      <c r="W7" s="205"/>
+      <c r="U7" s="250"/>
+      <c r="V7" s="250"/>
+      <c r="W7" s="251"/>
       <c r="X7" s="2"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
-      <c r="B8" s="230" t="e">
+      <c r="B8" s="231" t="e">
         <f>IF(CorrectionParameters_Temperature_Active,"Déflexions corrigées de :","Déflexions non corrigées")</f>
         <v>#NAME?</v>
       </c>
-      <c r="C8" s="231"/>
-      <c r="D8" s="231"/>
+      <c r="C8" s="232"/>
+      <c r="D8" s="232"/>
       <c r="E8" s="95" t="e">
         <f>IF(CorrectionParameters_Temperature_Active,_xlfn.SWITCH(CorrectionParameters_Temperature_TemperatureFromSource,"Tair",AVERAGE(Zi_Pi_Tair),"Tsurf",AVERAGE(Zi_Pi_Tsurf),"Tman",AVERAGE(Zi_Pi_Tman),"Custom",CorrectionParameters_Temperature_CustomValue),"")</f>
         <v>#NAME?</v>
@@ -9746,18 +9764,18 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
-      <c r="B9" s="232" t="e">
+      <c r="B9" s="233" t="e">
         <f>IF(CorrectionParameters_Temperature_Active,"Type de structure :","")</f>
         <v>#NAME?</v>
       </c>
-      <c r="C9" s="233"/>
-      <c r="D9" s="233"/>
-      <c r="E9" s="237" t="e">
+      <c r="C9" s="234"/>
+      <c r="D9" s="234"/>
+      <c r="E9" s="238" t="e">
         <f>IF(CorrectionParameters_Temperature_Active,CorrectionParameters_Temperature_StructureType_Name &amp; " K=" &amp; ROUND(CorrectionParameters_Temperature_StructureType_K,2),"")</f>
         <v>#NAME?</v>
       </c>
-      <c r="F9" s="237"/>
-      <c r="G9" s="237"/>
+      <c r="F9" s="238"/>
+      <c r="G9" s="238"/>
       <c r="H9" s="97"/>
       <c r="I9" s="39"/>
       <c r="J9" s="39"/>
@@ -9812,69 +9830,69 @@
     </row>
     <row r="11" spans="1:24" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
-      <c r="B11" s="186" t="s">
+      <c r="B11" s="188" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="187"/>
-      <c r="D11" s="187"/>
-      <c r="E11" s="187"/>
-      <c r="F11" s="187"/>
-      <c r="G11" s="187"/>
-      <c r="H11" s="187"/>
-      <c r="I11" s="187"/>
-      <c r="J11" s="187"/>
-      <c r="K11" s="187"/>
-      <c r="L11" s="187"/>
-      <c r="M11" s="187"/>
-      <c r="N11" s="187"/>
-      <c r="O11" s="187"/>
-      <c r="P11" s="187"/>
-      <c r="Q11" s="187"/>
-      <c r="R11" s="187"/>
-      <c r="S11" s="187"/>
-      <c r="T11" s="187"/>
-      <c r="U11" s="187"/>
-      <c r="V11" s="187"/>
-      <c r="W11" s="188"/>
+      <c r="C11" s="189"/>
+      <c r="D11" s="189"/>
+      <c r="E11" s="189"/>
+      <c r="F11" s="189"/>
+      <c r="G11" s="189"/>
+      <c r="H11" s="189"/>
+      <c r="I11" s="189"/>
+      <c r="J11" s="189"/>
+      <c r="K11" s="189"/>
+      <c r="L11" s="189"/>
+      <c r="M11" s="189"/>
+      <c r="N11" s="189"/>
+      <c r="O11" s="189"/>
+      <c r="P11" s="189"/>
+      <c r="Q11" s="189"/>
+      <c r="R11" s="189"/>
+      <c r="S11" s="189"/>
+      <c r="T11" s="189"/>
+      <c r="U11" s="189"/>
+      <c r="V11" s="189"/>
+      <c r="W11" s="190"/>
       <c r="X11" s="2"/>
     </row>
     <row r="12" spans="1:24" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="238"/>
+      <c r="A12" s="239"/>
       <c r="B12" s="63"/>
-      <c r="C12" s="239" t="s">
+      <c r="C12" s="240" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="240"/>
-      <c r="E12" s="241"/>
-      <c r="F12" s="239" t="s">
+      <c r="D12" s="241"/>
+      <c r="E12" s="242"/>
+      <c r="F12" s="240" t="s">
         <v>56</v>
       </c>
-      <c r="G12" s="240"/>
-      <c r="H12" s="239" t="e" cm="1">
+      <c r="G12" s="241"/>
+      <c r="H12" s="240" t="e" cm="1">
         <f t="array" ref="H12">CONCATENATE("Deflexion (",Unit_Deflection_Unit,") :")</f>
         <v>#NAME?</v>
       </c>
-      <c r="I12" s="240"/>
-      <c r="J12" s="240"/>
-      <c r="K12" s="240"/>
-      <c r="L12" s="240"/>
-      <c r="M12" s="240"/>
-      <c r="N12" s="240"/>
-      <c r="O12" s="240"/>
-      <c r="P12" s="240"/>
-      <c r="Q12" s="240"/>
-      <c r="R12" s="240"/>
-      <c r="S12" s="241"/>
+      <c r="I12" s="241"/>
+      <c r="J12" s="241"/>
+      <c r="K12" s="241"/>
+      <c r="L12" s="241"/>
+      <c r="M12" s="241"/>
+      <c r="N12" s="241"/>
+      <c r="O12" s="241"/>
+      <c r="P12" s="241"/>
+      <c r="Q12" s="241"/>
+      <c r="R12" s="241"/>
+      <c r="S12" s="242"/>
       <c r="T12" s="64"/>
-      <c r="U12" s="242" t="s">
+      <c r="U12" s="243" t="s">
         <v>57</v>
       </c>
-      <c r="V12" s="243"/>
-      <c r="W12" s="244"/>
+      <c r="V12" s="244"/>
+      <c r="W12" s="245"/>
       <c r="X12" s="19"/>
     </row>
     <row r="13" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="238"/>
+      <c r="A13" s="239"/>
       <c r="B13" s="65" t="s">
         <v>58</v>
       </c>
@@ -9932,9 +9950,9 @@
       <c r="T13" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="U13" s="245"/>
-      <c r="V13" s="246"/>
-      <c r="W13" s="247"/>
+      <c r="U13" s="246"/>
+      <c r="V13" s="247"/>
+      <c r="W13" s="248"/>
       <c r="X13" s="2"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.3">
@@ -9997,9 +10015,9 @@
       <c r="T14" s="76" t="s">
         <v>80</v>
       </c>
-      <c r="U14" s="234"/>
-      <c r="V14" s="235"/>
-      <c r="W14" s="236"/>
+      <c r="U14" s="235"/>
+      <c r="V14" s="236"/>
+      <c r="W14" s="237"/>
       <c r="X14" s="2"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.3">
@@ -10026,9 +10044,9 @@
       <c r="R15" s="87"/>
       <c r="S15" s="87"/>
       <c r="T15" s="76"/>
-      <c r="U15" s="227"/>
-      <c r="V15" s="228"/>
-      <c r="W15" s="229"/>
+      <c r="U15" s="228"/>
+      <c r="V15" s="229"/>
+      <c r="W15" s="230"/>
       <c r="X15" s="2"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.3">
@@ -10055,9 +10073,9 @@
       <c r="R16" s="87"/>
       <c r="S16" s="87"/>
       <c r="T16" s="83"/>
-      <c r="U16" s="227"/>
-      <c r="V16" s="228"/>
-      <c r="W16" s="229"/>
+      <c r="U16" s="228"/>
+      <c r="V16" s="229"/>
+      <c r="W16" s="230"/>
       <c r="X16" s="2"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.3">
@@ -10084,9 +10102,9 @@
       <c r="R17" s="87"/>
       <c r="S17" s="87"/>
       <c r="T17" s="83"/>
-      <c r="U17" s="227"/>
-      <c r="V17" s="228"/>
-      <c r="W17" s="229"/>
+      <c r="U17" s="228"/>
+      <c r="V17" s="229"/>
+      <c r="W17" s="230"/>
       <c r="X17" s="2"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.3">
@@ -10113,9 +10131,9 @@
       <c r="R18" s="87"/>
       <c r="S18" s="87"/>
       <c r="T18" s="83"/>
-      <c r="U18" s="227"/>
-      <c r="V18" s="228"/>
-      <c r="W18" s="229"/>
+      <c r="U18" s="228"/>
+      <c r="V18" s="229"/>
+      <c r="W18" s="230"/>
       <c r="X18" s="2"/>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.3">
@@ -10345,9 +10363,9 @@
       <c r="R26" s="87"/>
       <c r="S26" s="87"/>
       <c r="T26" s="83"/>
-      <c r="U26" s="227"/>
-      <c r="V26" s="228"/>
-      <c r="W26" s="229"/>
+      <c r="U26" s="228"/>
+      <c r="V26" s="229"/>
+      <c r="W26" s="230"/>
       <c r="X26" s="2"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.3">
@@ -10374,9 +10392,9 @@
       <c r="R27" s="87"/>
       <c r="S27" s="87"/>
       <c r="T27" s="83"/>
-      <c r="U27" s="227"/>
-      <c r="V27" s="228"/>
-      <c r="W27" s="229"/>
+      <c r="U27" s="228"/>
+      <c r="V27" s="229"/>
+      <c r="W27" s="230"/>
       <c r="X27" s="2"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.3">
@@ -10403,9 +10421,9 @@
       <c r="R28" s="87"/>
       <c r="S28" s="87"/>
       <c r="T28" s="83"/>
-      <c r="U28" s="227"/>
-      <c r="V28" s="228"/>
-      <c r="W28" s="229"/>
+      <c r="U28" s="228"/>
+      <c r="V28" s="229"/>
+      <c r="W28" s="230"/>
       <c r="X28" s="2"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.3">
@@ -10432,9 +10450,9 @@
       <c r="R29" s="87"/>
       <c r="S29" s="87"/>
       <c r="T29" s="83"/>
-      <c r="U29" s="227"/>
-      <c r="V29" s="228"/>
-      <c r="W29" s="229"/>
+      <c r="U29" s="228"/>
+      <c r="V29" s="229"/>
+      <c r="W29" s="230"/>
       <c r="X29" s="2"/>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.3">
@@ -10458,9 +10476,9 @@
       <c r="R30" s="87"/>
       <c r="S30" s="87"/>
       <c r="T30" s="83"/>
-      <c r="U30" s="227"/>
-      <c r="V30" s="228"/>
-      <c r="W30" s="229"/>
+      <c r="U30" s="228"/>
+      <c r="V30" s="229"/>
+      <c r="W30" s="230"/>
       <c r="X30" s="2"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.3">
@@ -10545,9 +10563,9 @@
       <c r="R33" s="87"/>
       <c r="S33" s="87"/>
       <c r="T33" s="83"/>
-      <c r="U33" s="227"/>
-      <c r="V33" s="228"/>
-      <c r="W33" s="229"/>
+      <c r="U33" s="228"/>
+      <c r="V33" s="229"/>
+      <c r="W33" s="230"/>
       <c r="X33" s="2"/>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.3">
@@ -10574,9 +10592,9 @@
       <c r="R34" s="87"/>
       <c r="S34" s="87"/>
       <c r="T34" s="83"/>
-      <c r="U34" s="227"/>
-      <c r="V34" s="228"/>
-      <c r="W34" s="229"/>
+      <c r="U34" s="228"/>
+      <c r="V34" s="229"/>
+      <c r="W34" s="230"/>
       <c r="X34" s="2"/>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.3">
@@ -10603,9 +10621,9 @@
       <c r="R35" s="87"/>
       <c r="S35" s="87"/>
       <c r="T35" s="83"/>
-      <c r="U35" s="227"/>
-      <c r="V35" s="228"/>
-      <c r="W35" s="229"/>
+      <c r="U35" s="228"/>
+      <c r="V35" s="229"/>
+      <c r="W35" s="230"/>
       <c r="X35" s="2"/>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.3">
@@ -10638,58 +10656,58 @@
       <c r="A37" s="2"/>
       <c r="B37" s="27"/>
       <c r="C37" s="27"/>
-      <c r="D37" s="172" t="s">
+      <c r="D37" s="174" t="s">
         <v>39</v>
       </c>
-      <c r="E37" s="172"/>
-      <c r="F37" s="172"/>
-      <c r="G37" s="172"/>
-      <c r="H37" s="172"/>
-      <c r="I37" s="172"/>
-      <c r="J37" s="172"/>
-      <c r="K37" s="172"/>
-      <c r="L37" s="172"/>
-      <c r="M37" s="172"/>
-      <c r="N37" s="172"/>
-      <c r="O37" s="172"/>
-      <c r="P37" s="172"/>
-      <c r="Q37" s="172"/>
-      <c r="R37" s="172"/>
-      <c r="S37" s="172"/>
-      <c r="T37" s="172"/>
-      <c r="U37" s="172"/>
-      <c r="V37" s="173" t="s">
+      <c r="E37" s="174"/>
+      <c r="F37" s="174"/>
+      <c r="G37" s="174"/>
+      <c r="H37" s="174"/>
+      <c r="I37" s="174"/>
+      <c r="J37" s="174"/>
+      <c r="K37" s="174"/>
+      <c r="L37" s="174"/>
+      <c r="M37" s="174"/>
+      <c r="N37" s="174"/>
+      <c r="O37" s="174"/>
+      <c r="P37" s="174"/>
+      <c r="Q37" s="174"/>
+      <c r="R37" s="174"/>
+      <c r="S37" s="174"/>
+      <c r="T37" s="174"/>
+      <c r="U37" s="174"/>
+      <c r="V37" s="175" t="s">
         <v>34</v>
       </c>
-      <c r="W37" s="173"/>
+      <c r="W37" s="175"/>
       <c r="X37" s="2"/>
     </row>
     <row r="38" spans="1:24" ht="11.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
-      <c r="D38" s="175" t="s">
+      <c r="D38" s="177" t="s">
         <v>40</v>
       </c>
-      <c r="E38" s="175"/>
-      <c r="F38" s="175"/>
-      <c r="G38" s="175"/>
-      <c r="H38" s="175"/>
-      <c r="I38" s="175"/>
-      <c r="J38" s="175"/>
-      <c r="K38" s="175"/>
-      <c r="L38" s="175"/>
-      <c r="M38" s="175"/>
-      <c r="N38" s="175"/>
-      <c r="O38" s="175"/>
-      <c r="P38" s="175"/>
-      <c r="Q38" s="175"/>
-      <c r="R38" s="175"/>
-      <c r="S38" s="175"/>
-      <c r="T38" s="175"/>
-      <c r="U38" s="175"/>
-      <c r="V38" s="174"/>
-      <c r="W38" s="174"/>
+      <c r="E38" s="177"/>
+      <c r="F38" s="177"/>
+      <c r="G38" s="177"/>
+      <c r="H38" s="177"/>
+      <c r="I38" s="177"/>
+      <c r="J38" s="177"/>
+      <c r="K38" s="177"/>
+      <c r="L38" s="177"/>
+      <c r="M38" s="177"/>
+      <c r="N38" s="177"/>
+      <c r="O38" s="177"/>
+      <c r="P38" s="177"/>
+      <c r="Q38" s="177"/>
+      <c r="R38" s="177"/>
+      <c r="S38" s="177"/>
+      <c r="T38" s="177"/>
+      <c r="U38" s="177"/>
+      <c r="V38" s="176"/>
+      <c r="W38" s="176"/>
       <c r="X38" s="2"/>
     </row>
   </sheetData>
@@ -10740,8 +10758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D79D983D-0860-4B05-AFF1-840CC1A0D13C}">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" view="pageLayout" zoomScaleNormal="115" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScaleNormal="115" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -10776,17 +10794,17 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="248" t="s">
+      <c r="E2" s="249" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="248"/>
-      <c r="G2" s="248"/>
-      <c r="H2" s="248"/>
-      <c r="I2" s="248"/>
-      <c r="J2" s="248"/>
-      <c r="K2" s="248"/>
-      <c r="L2" s="248"/>
-      <c r="M2" s="248"/>
+      <c r="F2" s="249"/>
+      <c r="G2" s="249"/>
+      <c r="H2" s="249"/>
+      <c r="I2" s="249"/>
+      <c r="J2" s="249"/>
+      <c r="K2" s="249"/>
+      <c r="L2" s="249"/>
+      <c r="M2" s="249"/>
       <c r="N2" s="150"/>
       <c r="O2" s="2"/>
     </row>
@@ -10795,17 +10813,17 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="215" t="s">
+      <c r="E3" s="216" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="215"/>
-      <c r="G3" s="215"/>
-      <c r="H3" s="215"/>
-      <c r="I3" s="215"/>
-      <c r="J3" s="215"/>
-      <c r="K3" s="215"/>
-      <c r="L3" s="215"/>
-      <c r="M3" s="215"/>
+      <c r="F3" s="216"/>
+      <c r="G3" s="216"/>
+      <c r="H3" s="216"/>
+      <c r="I3" s="216"/>
+      <c r="J3" s="216"/>
+      <c r="K3" s="216"/>
+      <c r="L3" s="216"/>
+      <c r="M3" s="216"/>
       <c r="N3" s="4"/>
       <c r="O3" s="2"/>
     </row>
@@ -10827,17 +10845,17 @@
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="218"/>
-      <c r="B5" s="218"/>
-      <c r="C5" s="218"/>
-      <c r="D5" s="218"/>
-      <c r="E5" s="218"/>
-      <c r="F5" s="218"/>
-      <c r="G5" s="218"/>
-      <c r="H5" s="218"/>
-      <c r="I5" s="218"/>
-      <c r="J5" s="218"/>
-      <c r="K5" s="218"/>
+      <c r="A5" s="219"/>
+      <c r="B5" s="219"/>
+      <c r="C5" s="219"/>
+      <c r="D5" s="219"/>
+      <c r="E5" s="219"/>
+      <c r="F5" s="219"/>
+      <c r="G5" s="219"/>
+      <c r="H5" s="219"/>
+      <c r="I5" s="219"/>
+      <c r="J5" s="219"/>
+      <c r="K5" s="219"/>
       <c r="L5" s="59"/>
       <c r="M5" s="59"/>
       <c r="N5" s="2"/>
@@ -10845,32 +10863,32 @@
     </row>
     <row r="6" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
-      <c r="B6" s="186" t="e" cm="1">
+      <c r="B6" s="188" t="e" cm="1">
         <f t="array" ref="B6" xml:space="preserve"> "INFORMATIONS ZONE " &amp; Zi_Name</f>
         <v>#NAME?</v>
       </c>
-      <c r="C6" s="187"/>
-      <c r="D6" s="187"/>
-      <c r="E6" s="187"/>
-      <c r="F6" s="187"/>
-      <c r="G6" s="187"/>
-      <c r="H6" s="187"/>
-      <c r="I6" s="187"/>
-      <c r="J6" s="187"/>
-      <c r="K6" s="187"/>
-      <c r="L6" s="187"/>
-      <c r="M6" s="187"/>
-      <c r="N6" s="188"/>
+      <c r="C6" s="189"/>
+      <c r="D6" s="189"/>
+      <c r="E6" s="189"/>
+      <c r="F6" s="189"/>
+      <c r="G6" s="189"/>
+      <c r="H6" s="189"/>
+      <c r="I6" s="189"/>
+      <c r="J6" s="189"/>
+      <c r="K6" s="189"/>
+      <c r="L6" s="189"/>
+      <c r="M6" s="189"/>
+      <c r="N6" s="190"/>
       <c r="O6" s="2"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
-      <c r="B7" s="249" t="e">
+      <c r="B7" s="252" t="e">
         <f>IF(CorrectionParameters_Load_Active,"Forces corrigées à :","Forces non corrigées")</f>
         <v>#NAME?</v>
       </c>
-      <c r="C7" s="250"/>
-      <c r="D7" s="250"/>
+      <c r="C7" s="253"/>
+      <c r="D7" s="253"/>
       <c r="E7" s="29" t="e">
         <f>IF(CorrectionParameters_Load_Active,IF(CorrectionParameters_Load_LoadReferenceSource="Sequence",DropSequence_Drop3_Value,CorrectionParameters_Load_CustomValue),"")</f>
         <v>#NAME?</v>
@@ -10883,25 +10901,25 @@
       <c r="H7" s="5"/>
       <c r="I7" s="31"/>
       <c r="J7" s="31"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5" t="s">
+      <c r="K7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="31" t="e">
+      <c r="L7" s="31" t="e">
         <f>IF(Project_Name="","",Project_Name)</f>
         <v>#NAME?</v>
       </c>
-      <c r="N7" s="41"/>
+      <c r="M7" s="269"/>
+      <c r="N7" s="271"/>
       <c r="O7" s="2"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
-      <c r="B8" s="230" t="e">
+      <c r="B8" s="231" t="e">
         <f>IF(CorrectionParameters_Temperature_Active,"Déflexions corrigées de :","Déflexions non corrigées")</f>
         <v>#NAME?</v>
       </c>
-      <c r="C8" s="231"/>
-      <c r="D8" s="231"/>
+      <c r="C8" s="232"/>
+      <c r="D8" s="232"/>
       <c r="E8" s="168" t="e">
         <f>IF(CorrectionParameters_Temperature_Active,_xlfn.SWITCH(CorrectionParameters_Temperature_TemperatureFromSource,"Tair",AVERAGE(Zi_Pi_Tair),"Tsurf",AVERAGE(Zi_Pi_Tsurf),"Tman",AVERAGE(Zi_Pi_Tman),"Custom",CorrectionParameters_Temperature_CustomValue),"")</f>
         <v>#NAME?</v>
@@ -10917,49 +10935,49 @@
       <c r="H8" s="46"/>
       <c r="I8" s="34"/>
       <c r="J8" s="34"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="101" t="s">
+      <c r="K8" s="101" t="s">
         <v>95</v>
       </c>
-      <c r="M8" s="131" t="str">
+      <c r="L8" s="131" t="str">
         <f>IFERROR(AVERAGE(Z1_Pi_D3_D0),"")</f>
         <v/>
       </c>
-      <c r="N8" s="99" t="e" cm="1">
-        <f t="array" ref="N8">Unit_Deflection_Unit</f>
-        <v>#NAME?</v>
-      </c>
+      <c r="M8" s="270" t="e" cm="1">
+        <f t="array" ref="M8">Unit_Deflection_Unit</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N8" s="99"/>
       <c r="O8" s="2"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
-      <c r="B9" s="232" t="e">
+      <c r="B9" s="233" t="e">
         <f>IF(CorrectionParameters_Temperature_Active,"Type de structure :","")</f>
         <v>#NAME?</v>
       </c>
-      <c r="C9" s="233"/>
-      <c r="D9" s="233"/>
-      <c r="E9" s="237" t="e">
+      <c r="C9" s="234"/>
+      <c r="D9" s="234"/>
+      <c r="E9" s="238" t="e">
         <f>IF(CorrectionParameters_Temperature_Active,CorrectionParameters_Temperature_StructureType_Name &amp; " K=" &amp; ROUND(CorrectionParameters_Temperature_StructureType_K,2),"")</f>
         <v>#NAME?</v>
       </c>
-      <c r="F9" s="237"/>
-      <c r="G9" s="237"/>
+      <c r="F9" s="238"/>
+      <c r="G9" s="238"/>
       <c r="H9" s="97"/>
       <c r="I9" s="39"/>
       <c r="J9" s="39"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="96" t="s">
+      <c r="K9" s="96" t="s">
         <v>96</v>
       </c>
-      <c r="M9" s="132" t="str" cm="1">
-        <f t="array" ref="M9">IFERROR(Zi_CharacteristicDeflection,"")</f>
-        <v/>
-      </c>
-      <c r="N9" s="100" t="e" cm="1">
-        <f t="array" ref="N9">Unit_Deflection_Unit</f>
-        <v>#NAME?</v>
-      </c>
+      <c r="L9" s="132" t="str" cm="1">
+        <f t="array" ref="L9">IFERROR(Zi_CharacteristicDeflection,"")</f>
+        <v/>
+      </c>
+      <c r="M9" s="98" t="e" cm="1">
+        <f t="array" ref="M9">Unit_Deflection_Unit</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N9" s="100"/>
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -10981,51 +10999,51 @@
     </row>
     <row r="11" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
-      <c r="B11" s="186" t="s">
+      <c r="B11" s="188" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="187"/>
-      <c r="D11" s="187"/>
-      <c r="E11" s="187"/>
-      <c r="F11" s="187"/>
-      <c r="G11" s="187"/>
-      <c r="H11" s="187"/>
-      <c r="I11" s="187"/>
-      <c r="J11" s="187"/>
-      <c r="K11" s="187"/>
-      <c r="L11" s="187"/>
-      <c r="M11" s="187"/>
-      <c r="N11" s="188"/>
+      <c r="C11" s="189"/>
+      <c r="D11" s="189"/>
+      <c r="E11" s="189"/>
+      <c r="F11" s="189"/>
+      <c r="G11" s="189"/>
+      <c r="H11" s="189"/>
+      <c r="I11" s="189"/>
+      <c r="J11" s="189"/>
+      <c r="K11" s="189"/>
+      <c r="L11" s="189"/>
+      <c r="M11" s="189"/>
+      <c r="N11" s="190"/>
       <c r="O11" s="2"/>
     </row>
     <row r="12" spans="1:15" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="238"/>
+      <c r="A12" s="239"/>
       <c r="B12" s="63"/>
-      <c r="C12" s="239" t="s">
+      <c r="C12" s="240" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="240"/>
-      <c r="E12" s="241"/>
-      <c r="F12" s="239" t="s">
+      <c r="D12" s="241"/>
+      <c r="E12" s="242"/>
+      <c r="F12" s="240" t="s">
         <v>56</v>
       </c>
-      <c r="G12" s="240"/>
-      <c r="H12" s="239" t="e" cm="1">
+      <c r="G12" s="241"/>
+      <c r="H12" s="240" t="e" cm="1">
         <f t="array" ref="H12">CONCATENATE("Deflexion (",Unit_Deflection_Unit,") :")</f>
         <v>#NAME?</v>
       </c>
-      <c r="I12" s="240"/>
-      <c r="J12" s="240"/>
-      <c r="K12" s="240"/>
-      <c r="L12" s="240"/>
-      <c r="M12" s="239" t="s">
+      <c r="I12" s="241"/>
+      <c r="J12" s="241"/>
+      <c r="K12" s="241"/>
+      <c r="L12" s="241"/>
+      <c r="M12" s="240" t="s">
         <v>176</v>
       </c>
-      <c r="N12" s="251"/>
+      <c r="N12" s="254"/>
       <c r="O12" s="19"/>
     </row>
     <row r="13" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="238"/>
+      <c r="A13" s="239"/>
       <c r="B13" s="65" t="s">
         <v>58</v>
       </c>
@@ -11889,18 +11907,18 @@
       <c r="A54" s="2"/>
       <c r="B54" s="27"/>
       <c r="C54" s="27"/>
-      <c r="D54" s="172" t="s">
+      <c r="D54" s="174" t="s">
         <v>39</v>
       </c>
-      <c r="E54" s="172"/>
-      <c r="F54" s="172"/>
-      <c r="G54" s="172"/>
-      <c r="H54" s="172"/>
-      <c r="I54" s="172"/>
-      <c r="J54" s="172"/>
-      <c r="K54" s="172"/>
-      <c r="L54" s="172"/>
-      <c r="M54" s="172"/>
+      <c r="E54" s="174"/>
+      <c r="F54" s="174"/>
+      <c r="G54" s="174"/>
+      <c r="H54" s="174"/>
+      <c r="I54" s="174"/>
+      <c r="J54" s="174"/>
+      <c r="K54" s="174"/>
+      <c r="L54" s="174"/>
+      <c r="M54" s="174"/>
       <c r="N54" s="165" t="s">
         <v>34</v>
       </c>
@@ -11910,18 +11928,18 @@
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
-      <c r="D55" s="175" t="s">
+      <c r="D55" s="177" t="s">
         <v>40</v>
       </c>
-      <c r="E55" s="175"/>
-      <c r="F55" s="175"/>
-      <c r="G55" s="175"/>
-      <c r="H55" s="175"/>
-      <c r="I55" s="175"/>
-      <c r="J55" s="175"/>
-      <c r="K55" s="175"/>
-      <c r="L55" s="175"/>
-      <c r="M55" s="175"/>
+      <c r="E55" s="177"/>
+      <c r="F55" s="177"/>
+      <c r="G55" s="177"/>
+      <c r="H55" s="177"/>
+      <c r="I55" s="177"/>
+      <c r="J55" s="177"/>
+      <c r="K55" s="177"/>
+      <c r="L55" s="177"/>
+      <c r="M55" s="177"/>
       <c r="N55" s="164"/>
       <c r="O55" s="2"/>
     </row>
@@ -12057,13 +12075,13 @@
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="218"/>
-      <c r="B5" s="218"/>
-      <c r="C5" s="218"/>
-      <c r="D5" s="218"/>
-      <c r="E5" s="218"/>
-      <c r="F5" s="218"/>
-      <c r="G5" s="218"/>
+      <c r="A5" s="219"/>
+      <c r="B5" s="219"/>
+      <c r="C5" s="219"/>
+      <c r="D5" s="219"/>
+      <c r="E5" s="219"/>
+      <c r="F5" s="219"/>
+      <c r="G5" s="219"/>
       <c r="H5" s="59"/>
       <c r="I5" s="59"/>
       <c r="J5" s="59"/>
@@ -12078,24 +12096,24 @@
     </row>
     <row r="6" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
-      <c r="B6" s="186" t="s">
+      <c r="B6" s="188" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="187"/>
-      <c r="D6" s="187"/>
-      <c r="E6" s="187"/>
-      <c r="F6" s="187"/>
-      <c r="G6" s="187"/>
-      <c r="H6" s="187"/>
-      <c r="I6" s="187"/>
-      <c r="J6" s="187"/>
-      <c r="K6" s="187"/>
-      <c r="L6" s="187"/>
-      <c r="M6" s="187"/>
-      <c r="N6" s="187"/>
-      <c r="O6" s="187"/>
-      <c r="P6" s="187"/>
-      <c r="Q6" s="188"/>
+      <c r="C6" s="189"/>
+      <c r="D6" s="189"/>
+      <c r="E6" s="189"/>
+      <c r="F6" s="189"/>
+      <c r="G6" s="189"/>
+      <c r="H6" s="189"/>
+      <c r="I6" s="189"/>
+      <c r="J6" s="189"/>
+      <c r="K6" s="189"/>
+      <c r="L6" s="189"/>
+      <c r="M6" s="189"/>
+      <c r="N6" s="189"/>
+      <c r="O6" s="189"/>
+      <c r="P6" s="189"/>
+      <c r="Q6" s="190"/>
       <c r="R6" s="2"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
@@ -12104,23 +12122,23 @@
       <c r="C7" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="252" t="e">
+      <c r="D7" s="255" t="e">
         <f>IF(Project_Name="","",Project_Name)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E7" s="252"/>
-      <c r="F7" s="252"/>
+      <c r="E7" s="255"/>
+      <c r="F7" s="255"/>
       <c r="G7" s="61"/>
       <c r="H7" s="107"/>
       <c r="I7" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="255">
+      <c r="J7" s="258">
         <f ca="1">TODAY()</f>
-        <v>44984</v>
-      </c>
-      <c r="K7" s="255"/>
-      <c r="L7" s="255"/>
+        <v>44993</v>
+      </c>
+      <c r="K7" s="258"/>
+      <c r="L7" s="258"/>
       <c r="M7" s="29"/>
       <c r="N7" s="29"/>
       <c r="O7" s="29"/>
@@ -12134,23 +12152,23 @@
       <c r="C8" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="253" t="e">
+      <c r="D8" s="256" t="e">
         <f>IF(Project_Town="","",Project_Town)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E8" s="253"/>
-      <c r="F8" s="253"/>
+      <c r="E8" s="256"/>
+      <c r="F8" s="256"/>
       <c r="G8" s="111"/>
       <c r="H8" s="112"/>
       <c r="I8" s="111" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="256" t="e">
+      <c r="J8" s="259" t="e">
         <f>IF(Report_Date="","",Report_Date)</f>
         <v>#NAME?</v>
       </c>
-      <c r="K8" s="256"/>
-      <c r="L8" s="256"/>
+      <c r="K8" s="259"/>
+      <c r="L8" s="259"/>
       <c r="M8" s="40"/>
       <c r="N8" s="40"/>
       <c r="O8" s="40"/>
@@ -12164,23 +12182,23 @@
       <c r="C9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="254" t="e">
+      <c r="D9" s="257" t="e">
         <f>IF(Project_Customer="","",Project_Customer)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E9" s="254"/>
-      <c r="F9" s="254"/>
+      <c r="E9" s="257"/>
+      <c r="F9" s="257"/>
       <c r="G9" s="14"/>
       <c r="H9" s="117"/>
       <c r="I9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="257" t="e">
+      <c r="J9" s="260" t="e">
         <f>IF(Project_Project="","", Project_Project)</f>
         <v>#NAME?</v>
       </c>
-      <c r="K9" s="257"/>
-      <c r="L9" s="257"/>
+      <c r="K9" s="260"/>
+      <c r="L9" s="260"/>
       <c r="M9" s="55"/>
       <c r="N9" s="55"/>
       <c r="O9" s="55"/>
@@ -12772,46 +12790,46 @@
       <c r="A39" s="2"/>
       <c r="B39" s="27"/>
       <c r="C39" s="27"/>
-      <c r="D39" s="172" t="s">
+      <c r="D39" s="174" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="172"/>
-      <c r="F39" s="172"/>
-      <c r="G39" s="172"/>
-      <c r="H39" s="172"/>
-      <c r="I39" s="172"/>
-      <c r="J39" s="172"/>
-      <c r="K39" s="172"/>
-      <c r="L39" s="172"/>
-      <c r="M39" s="172"/>
-      <c r="N39" s="172"/>
-      <c r="O39" s="172"/>
-      <c r="P39" s="173" t="s">
+      <c r="E39" s="174"/>
+      <c r="F39" s="174"/>
+      <c r="G39" s="174"/>
+      <c r="H39" s="174"/>
+      <c r="I39" s="174"/>
+      <c r="J39" s="174"/>
+      <c r="K39" s="174"/>
+      <c r="L39" s="174"/>
+      <c r="M39" s="174"/>
+      <c r="N39" s="174"/>
+      <c r="O39" s="174"/>
+      <c r="P39" s="175" t="s">
         <v>34</v>
       </c>
-      <c r="Q39" s="173"/>
+      <c r="Q39" s="175"/>
       <c r="R39" s="2"/>
     </row>
     <row r="40" spans="1:18" ht="11.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
-      <c r="D40" s="175" t="s">
+      <c r="D40" s="177" t="s">
         <v>40</v>
       </c>
-      <c r="E40" s="175"/>
-      <c r="F40" s="175"/>
-      <c r="G40" s="175"/>
-      <c r="H40" s="175"/>
-      <c r="I40" s="175"/>
-      <c r="J40" s="175"/>
-      <c r="K40" s="175"/>
-      <c r="L40" s="175"/>
-      <c r="M40" s="175"/>
-      <c r="N40" s="175"/>
-      <c r="O40" s="175"/>
-      <c r="P40" s="174"/>
-      <c r="Q40" s="174"/>
+      <c r="E40" s="177"/>
+      <c r="F40" s="177"/>
+      <c r="G40" s="177"/>
+      <c r="H40" s="177"/>
+      <c r="I40" s="177"/>
+      <c r="J40" s="177"/>
+      <c r="K40" s="177"/>
+      <c r="L40" s="177"/>
+      <c r="M40" s="177"/>
+      <c r="N40" s="177"/>
+      <c r="O40" s="177"/>
+      <c r="P40" s="176"/>
+      <c r="Q40" s="176"/>
       <c r="R40" s="2"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.3">
@@ -16068,8 +16086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{095FCAD2-DD47-4982-BFBB-2918CDE0F2F3}">
   <dimension ref="A1:R500"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A38" zoomScaleNormal="115" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="O50" sqref="O50"/>
+    <sheetView showWhiteSpace="0" view="pageLayout" zoomScaleNormal="115" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -16167,13 +16185,13 @@
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="218"/>
-      <c r="B5" s="218"/>
-      <c r="C5" s="218"/>
-      <c r="D5" s="218"/>
-      <c r="E5" s="218"/>
-      <c r="F5" s="218"/>
-      <c r="G5" s="218"/>
+      <c r="A5" s="219"/>
+      <c r="B5" s="219"/>
+      <c r="C5" s="219"/>
+      <c r="D5" s="219"/>
+      <c r="E5" s="219"/>
+      <c r="F5" s="219"/>
+      <c r="G5" s="219"/>
       <c r="H5" s="59"/>
       <c r="I5" s="59"/>
       <c r="J5" s="59"/>
@@ -16188,24 +16206,24 @@
     </row>
     <row r="6" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
-      <c r="B6" s="186" t="s">
+      <c r="B6" s="188" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="187"/>
-      <c r="D6" s="187"/>
-      <c r="E6" s="187"/>
-      <c r="F6" s="187"/>
-      <c r="G6" s="187"/>
-      <c r="H6" s="187"/>
-      <c r="I6" s="187"/>
-      <c r="J6" s="187"/>
-      <c r="K6" s="187"/>
-      <c r="L6" s="187"/>
-      <c r="M6" s="187"/>
-      <c r="N6" s="187"/>
-      <c r="O6" s="187"/>
-      <c r="P6" s="187"/>
-      <c r="Q6" s="188"/>
+      <c r="C6" s="189"/>
+      <c r="D6" s="189"/>
+      <c r="E6" s="189"/>
+      <c r="F6" s="189"/>
+      <c r="G6" s="189"/>
+      <c r="H6" s="189"/>
+      <c r="I6" s="189"/>
+      <c r="J6" s="189"/>
+      <c r="K6" s="189"/>
+      <c r="L6" s="189"/>
+      <c r="M6" s="189"/>
+      <c r="N6" s="189"/>
+      <c r="O6" s="189"/>
+      <c r="P6" s="189"/>
+      <c r="Q6" s="190"/>
       <c r="R6" s="2"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
@@ -16214,23 +16232,23 @@
       <c r="C7" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="252" t="e">
+      <c r="D7" s="255" t="e">
         <f>IF(Project_Name="","",Project_Name)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E7" s="252"/>
-      <c r="F7" s="252"/>
+      <c r="E7" s="255"/>
+      <c r="F7" s="255"/>
       <c r="G7" s="61"/>
       <c r="H7" s="107"/>
       <c r="I7" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="255">
+      <c r="J7" s="258">
         <f ca="1">TODAY()</f>
-        <v>44984</v>
-      </c>
-      <c r="K7" s="255"/>
-      <c r="L7" s="255"/>
+        <v>44993</v>
+      </c>
+      <c r="K7" s="258"/>
+      <c r="L7" s="258"/>
       <c r="M7" s="29"/>
       <c r="N7" s="29"/>
       <c r="O7" s="29"/>
@@ -16244,23 +16262,23 @@
       <c r="C8" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="253" t="e">
+      <c r="D8" s="256" t="e">
         <f>IF(Project_Town="","",Project_Town)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E8" s="253"/>
-      <c r="F8" s="253"/>
+      <c r="E8" s="256"/>
+      <c r="F8" s="256"/>
       <c r="G8" s="111"/>
       <c r="H8" s="112"/>
       <c r="I8" s="111" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="256" t="e">
+      <c r="J8" s="259" t="e">
         <f>IF(Report_Date="","",Report_Date)</f>
         <v>#NAME?</v>
       </c>
-      <c r="K8" s="256"/>
-      <c r="L8" s="256"/>
+      <c r="K8" s="259"/>
+      <c r="L8" s="259"/>
       <c r="M8" s="40"/>
       <c r="N8" s="40"/>
       <c r="O8" s="40"/>
@@ -16274,23 +16292,23 @@
       <c r="C9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="254" t="e">
+      <c r="D9" s="257" t="e">
         <f>IF(Project_Customer="","",Project_Customer)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E9" s="254"/>
-      <c r="F9" s="254"/>
+      <c r="E9" s="257"/>
+      <c r="F9" s="257"/>
       <c r="G9" s="14"/>
       <c r="H9" s="117"/>
       <c r="I9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="257" t="e">
+      <c r="J9" s="260" t="e">
         <f>IF(Project_Project="","", Project_Project)</f>
         <v>#NAME?</v>
       </c>
-      <c r="K9" s="257"/>
-      <c r="L9" s="257"/>
+      <c r="K9" s="260"/>
+      <c r="L9" s="260"/>
       <c r="M9" s="55"/>
       <c r="N9" s="55"/>
       <c r="O9" s="55"/>
@@ -16882,46 +16900,46 @@
       <c r="A39" s="2"/>
       <c r="B39" s="27"/>
       <c r="C39" s="27"/>
-      <c r="D39" s="172" t="s">
+      <c r="D39" s="174" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="172"/>
-      <c r="F39" s="172"/>
-      <c r="G39" s="172"/>
-      <c r="H39" s="172"/>
-      <c r="I39" s="172"/>
-      <c r="J39" s="172"/>
-      <c r="K39" s="172"/>
-      <c r="L39" s="172"/>
-      <c r="M39" s="172"/>
-      <c r="N39" s="172"/>
-      <c r="O39" s="172"/>
-      <c r="P39" s="173" t="s">
+      <c r="E39" s="174"/>
+      <c r="F39" s="174"/>
+      <c r="G39" s="174"/>
+      <c r="H39" s="174"/>
+      <c r="I39" s="174"/>
+      <c r="J39" s="174"/>
+      <c r="K39" s="174"/>
+      <c r="L39" s="174"/>
+      <c r="M39" s="174"/>
+      <c r="N39" s="174"/>
+      <c r="O39" s="174"/>
+      <c r="P39" s="175" t="s">
         <v>34</v>
       </c>
-      <c r="Q39" s="173"/>
+      <c r="Q39" s="175"/>
       <c r="R39" s="2"/>
     </row>
     <row r="40" spans="1:18" ht="11.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
-      <c r="D40" s="175" t="s">
+      <c r="D40" s="177" t="s">
         <v>40</v>
       </c>
-      <c r="E40" s="175"/>
-      <c r="F40" s="175"/>
-      <c r="G40" s="175"/>
-      <c r="H40" s="175"/>
-      <c r="I40" s="175"/>
-      <c r="J40" s="175"/>
-      <c r="K40" s="175"/>
-      <c r="L40" s="175"/>
-      <c r="M40" s="175"/>
-      <c r="N40" s="175"/>
-      <c r="O40" s="175"/>
-      <c r="P40" s="174"/>
-      <c r="Q40" s="174"/>
+      <c r="E40" s="177"/>
+      <c r="F40" s="177"/>
+      <c r="G40" s="177"/>
+      <c r="H40" s="177"/>
+      <c r="I40" s="177"/>
+      <c r="J40" s="177"/>
+      <c r="K40" s="177"/>
+      <c r="L40" s="177"/>
+      <c r="M40" s="177"/>
+      <c r="N40" s="177"/>
+      <c r="O40" s="177"/>
+      <c r="P40" s="176"/>
+      <c r="Q40" s="176"/>
       <c r="R40" s="2"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.3">
@@ -25263,14 +25281,14 @@
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="262" t="s">
+      <c r="D2" s="265" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="262"/>
-      <c r="F2" s="262"/>
-      <c r="G2" s="262"/>
-      <c r="H2" s="262"/>
-      <c r="I2" s="262"/>
+      <c r="E2" s="265"/>
+      <c r="F2" s="265"/>
+      <c r="G2" s="265"/>
+      <c r="H2" s="265"/>
+      <c r="I2" s="265"/>
       <c r="J2" s="102"/>
     </row>
     <row r="3" spans="1:16" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
@@ -25301,46 +25319,46 @@
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="248" t="s">
+      <c r="D5" s="249" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="248"/>
-      <c r="F5" s="248"/>
-      <c r="G5" s="248"/>
-      <c r="H5" s="248"/>
-      <c r="I5" s="248"/>
-      <c r="J5" s="248"/>
+      <c r="E5" s="249"/>
+      <c r="F5" s="249"/>
+      <c r="G5" s="249"/>
+      <c r="H5" s="249"/>
+      <c r="I5" s="249"/>
+      <c r="J5" s="249"/>
     </row>
     <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="258"/>
-      <c r="B6" s="258"/>
-      <c r="C6" s="258"/>
-      <c r="D6" s="215" t="s">
+      <c r="A6" s="261"/>
+      <c r="B6" s="261"/>
+      <c r="C6" s="261"/>
+      <c r="D6" s="216" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="215"/>
-      <c r="F6" s="215"/>
-      <c r="G6" s="215"/>
-      <c r="H6" s="215"/>
-      <c r="I6" s="215"/>
-      <c r="J6" s="215"/>
+      <c r="E6" s="216"/>
+      <c r="F6" s="216"/>
+      <c r="G6" s="216"/>
+      <c r="H6" s="216"/>
+      <c r="I6" s="216"/>
+      <c r="J6" s="216"/>
     </row>
     <row r="7" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="258"/>
-      <c r="B7" s="258"/>
-      <c r="C7" s="258"/>
-      <c r="D7" s="215"/>
-      <c r="E7" s="215"/>
-      <c r="F7" s="215"/>
-      <c r="G7" s="215"/>
-      <c r="H7" s="215"/>
-      <c r="I7" s="215"/>
-      <c r="J7" s="215"/>
+      <c r="A7" s="261"/>
+      <c r="B7" s="261"/>
+      <c r="C7" s="261"/>
+      <c r="D7" s="216"/>
+      <c r="E7" s="216"/>
+      <c r="F7" s="216"/>
+      <c r="G7" s="216"/>
+      <c r="H7" s="216"/>
+      <c r="I7" s="216"/>
+      <c r="J7" s="216"/>
     </row>
     <row r="8" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="258"/>
-      <c r="B8" s="258"/>
-      <c r="C8" s="258"/>
+      <c r="A8" s="261"/>
+      <c r="B8" s="261"/>
+      <c r="C8" s="261"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -25350,9 +25368,9 @@
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="258"/>
-      <c r="B9" s="258"/>
-      <c r="C9" s="258"/>
+      <c r="A9" s="261"/>
+      <c r="B9" s="261"/>
+      <c r="C9" s="261"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="5"/>
@@ -25363,16 +25381,16 @@
     </row>
     <row r="10" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="103"/>
-      <c r="B10" s="259" t="s">
+      <c r="B10" s="262" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="260"/>
-      <c r="D10" s="260"/>
-      <c r="E10" s="260"/>
-      <c r="F10" s="260"/>
-      <c r="G10" s="260"/>
-      <c r="H10" s="260"/>
-      <c r="I10" s="261"/>
+      <c r="C10" s="263"/>
+      <c r="D10" s="263"/>
+      <c r="E10" s="263"/>
+      <c r="F10" s="263"/>
+      <c r="G10" s="263"/>
+      <c r="H10" s="263"/>
+      <c r="I10" s="264"/>
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -25393,7 +25411,7 @@
       </c>
       <c r="I11" s="107">
         <f ca="1">TODAY()</f>
-        <v>44984</v>
+        <v>44993</v>
       </c>
       <c r="J11" s="108"/>
     </row>
@@ -25455,16 +25473,16 @@
     </row>
     <row r="15" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="119"/>
-      <c r="B15" s="259" t="s">
+      <c r="B15" s="262" t="s">
         <v>97</v>
       </c>
-      <c r="C15" s="260"/>
-      <c r="D15" s="260"/>
-      <c r="E15" s="260"/>
-      <c r="F15" s="260"/>
-      <c r="G15" s="260"/>
-      <c r="H15" s="260"/>
-      <c r="I15" s="261"/>
+      <c r="C15" s="263"/>
+      <c r="D15" s="263"/>
+      <c r="E15" s="263"/>
+      <c r="F15" s="263"/>
+      <c r="G15" s="263"/>
+      <c r="H15" s="263"/>
+      <c r="I15" s="264"/>
       <c r="J15" s="120"/>
       <c r="M15" s="121"/>
       <c r="N15" s="121"/>
@@ -25942,42 +25960,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="B1" s="263" t="s">
+      <c r="B1" s="266" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="264"/>
-      <c r="D1" s="264"/>
-      <c r="E1" s="264"/>
-      <c r="F1" s="264"/>
-      <c r="G1" s="265"/>
-      <c r="H1" s="263" t="s">
+      <c r="C1" s="267"/>
+      <c r="D1" s="267"/>
+      <c r="E1" s="267"/>
+      <c r="F1" s="267"/>
+      <c r="G1" s="268"/>
+      <c r="H1" s="266" t="s">
         <v>135</v>
       </c>
-      <c r="I1" s="264"/>
-      <c r="J1" s="264"/>
-      <c r="K1" s="264"/>
-      <c r="L1" s="264"/>
-      <c r="M1" s="264"/>
-      <c r="N1" s="264"/>
-      <c r="O1" s="264"/>
-      <c r="P1" s="264"/>
-      <c r="Q1" s="264"/>
-      <c r="R1" s="264"/>
-      <c r="S1" s="264"/>
-      <c r="T1" s="265"/>
-      <c r="U1" s="264" t="s">
+      <c r="I1" s="267"/>
+      <c r="J1" s="267"/>
+      <c r="K1" s="267"/>
+      <c r="L1" s="267"/>
+      <c r="M1" s="267"/>
+      <c r="N1" s="267"/>
+      <c r="O1" s="267"/>
+      <c r="P1" s="267"/>
+      <c r="Q1" s="267"/>
+      <c r="R1" s="267"/>
+      <c r="S1" s="267"/>
+      <c r="T1" s="268"/>
+      <c r="U1" s="267" t="s">
         <v>136</v>
       </c>
-      <c r="V1" s="264"/>
-      <c r="W1" s="264"/>
-      <c r="X1" s="264"/>
-      <c r="Y1" s="264"/>
-      <c r="Z1" s="264"/>
-      <c r="AA1" s="264"/>
-      <c r="AB1" s="264"/>
-      <c r="AC1" s="264"/>
-      <c r="AD1" s="264"/>
-      <c r="AE1" s="264"/>
+      <c r="V1" s="267"/>
+      <c r="W1" s="267"/>
+      <c r="X1" s="267"/>
+      <c r="Y1" s="267"/>
+      <c r="Z1" s="267"/>
+      <c r="AA1" s="267"/>
+      <c r="AB1" s="267"/>
+      <c r="AC1" s="267"/>
+      <c r="AD1" s="267"/>
+      <c r="AE1" s="267"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A2" s="143" t="s">

</xml_diff>